<commit_message>
added separate swarm track
</commit_message>
<xml_diff>
--- a/Quotas.xlsx
+++ b/Quotas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\CloudContainerPlay\mschassis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A61222-CAB5-4AFC-96ED-A30074C15D87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529D01A9-CD99-47FC-A5CD-A0FC4F1112B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{04CF0484-DD32-4F74-AA83-46ADA1C4A4CA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>SERVICE</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>elk</t>
+  </si>
+  <si>
+    <t>Zookeeper + Each Broker</t>
+  </si>
+  <si>
+    <t>Master + Worker</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,11 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80665760-63A4-454E-B94B-31D9E3D15D31}">
-  <dimension ref="C1:E19"/>
+  <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,10 +500,11 @@
     <col min="3" max="3" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +515,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -512,7 +527,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
@@ -523,7 +539,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -534,7 +551,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
@@ -545,7 +563,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -556,7 +575,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
@@ -567,7 +587,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
@@ -578,7 +599,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
@@ -589,7 +611,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -600,7 +623,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -611,7 +635,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
@@ -621,8 +646,12 @@
       <c r="E12" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
@@ -633,7 +662,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
@@ -644,7 +674,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
@@ -654,8 +685,12 @@
       <c r="E15" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="4"/>
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
@@ -666,12 +701,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
@@ -682,7 +718,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C19" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>